<commit_message>
add dictionaries with hierarchies and period labels
</commit_message>
<xml_diff>
--- a/demo_order.xlsx
+++ b/demo_order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\!Projects\PG_portal\script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\d\Projects\!Projects\PG_portal\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7615A9-D688-48FC-8B8B-0F71F8433318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01AB584-6742-42C6-B1C5-FB3F1AA2E225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7C5B2639-0D78-4248-A766-610DD7AB3DE6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7C5B2639-0D78-4248-A766-610DD7AB3DE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>Buyer Group ID</t>
   </si>
@@ -232,6 +232,198 @@
   </si>
   <si>
     <t>demo_code</t>
+  </si>
+  <si>
+    <t>demo_hier</t>
+  </si>
+  <si>
+    <t>0. TOTAL DEMOGRAPHICS</t>
+  </si>
+  <si>
+    <t>1.1.0. 18-29 years</t>
+  </si>
+  <si>
+    <t>1.2.0. 30-39 years</t>
+  </si>
+  <si>
+    <t>1.3.0. 40-49 years</t>
+  </si>
+  <si>
+    <t>1.4.0. 50-59 years</t>
+  </si>
+  <si>
+    <t>1.5.0. 60+ years</t>
+  </si>
+  <si>
+    <t>2.1.0. 1</t>
+  </si>
+  <si>
+    <t>2.2.0. 2</t>
+  </si>
+  <si>
+    <t>2.3.0. 3</t>
+  </si>
+  <si>
+    <t>2.4.0. 4+</t>
+  </si>
+  <si>
+    <t>3.1.0. Children &lt;6 years</t>
+  </si>
+  <si>
+    <t>3.2.0. Children 6-14 years</t>
+  </si>
+  <si>
+    <t>3.3.0. Children 15-19 years</t>
+  </si>
+  <si>
+    <t>3.4.0. No Children &lt;20 years (Rest)</t>
+  </si>
+  <si>
+    <t>4.1.0. Employed full-time</t>
+  </si>
+  <si>
+    <t>4.2.0. Employed part-time</t>
+  </si>
+  <si>
+    <t>4.3.0. Not employed</t>
+  </si>
+  <si>
+    <t>5.1.0. Low Affluency</t>
+  </si>
+  <si>
+    <t>5.2.0. Below average affluency</t>
+  </si>
+  <si>
+    <t>5.3.0. Above average affluency</t>
+  </si>
+  <si>
+    <t>5.4.0. High affluency</t>
+  </si>
+  <si>
+    <t>6.1.0. Young singles/couples without</t>
+  </si>
+  <si>
+    <t>6.2.0. Mature singles/couples without</t>
+  </si>
+  <si>
+    <t>6.3.0. Senior singles/couples without</t>
+  </si>
+  <si>
+    <t>6.4.0. Retired singles/couples withou</t>
+  </si>
+  <si>
+    <t>6.5.0. Family with children &lt;18</t>
+  </si>
+  <si>
+    <t>6.5.1.0. Family with children &lt;6 years</t>
+  </si>
+  <si>
+    <t>6.5.1.1.0. Family with children 0-3 years</t>
+  </si>
+  <si>
+    <t>6.5.1.2.0. Family with children 4-5 years</t>
+  </si>
+  <si>
+    <t>6.5.2.0. Family with children 6-12 year</t>
+  </si>
+  <si>
+    <t>6.5.3.0. Family with children 13-18 yea</t>
+  </si>
+  <si>
+    <t>7.1.0. Moscow</t>
+  </si>
+  <si>
+    <t>7.2.0. St.Petersburg</t>
+  </si>
+  <si>
+    <t>7.3.0. 1mln+ population</t>
+  </si>
+  <si>
+    <t>7.4.0. 500 thd - 1 mln population</t>
+  </si>
+  <si>
+    <t>7.5.0. 10 thd - 500 thd population</t>
+  </si>
+  <si>
+    <t>7.6.0. Rural Area</t>
+  </si>
+  <si>
+    <t>8.1.0. &lt;10000 RBLS</t>
+  </si>
+  <si>
+    <t>8.2.0. 10001-45000 RBLS</t>
+  </si>
+  <si>
+    <t>8.3.0. 45001-60000 RBLS</t>
+  </si>
+  <si>
+    <t>8.4.0. &gt; 60000 RBLS</t>
+  </si>
+  <si>
+    <t>9.1.0. 0-12 month</t>
+  </si>
+  <si>
+    <t>9.2.0. 13-24 month</t>
+  </si>
+  <si>
+    <t>9.3.0. 25-36 month</t>
+  </si>
+  <si>
+    <t>8.1.0. No teen in HH</t>
+  </si>
+  <si>
+    <t>8.2.0. Teen girls 10 to 17 y.o</t>
+  </si>
+  <si>
+    <t>8.3.0. Teen girls 18 to 24 y.o</t>
+  </si>
+  <si>
+    <t>9.1.0. 18-24 yrs old</t>
+  </si>
+  <si>
+    <t>9.2.0. 25-34 yrs old</t>
+  </si>
+  <si>
+    <t>9.3.0. 35-49 yrs old</t>
+  </si>
+  <si>
+    <t>9.4.0. 50-64 yrs old</t>
+  </si>
+  <si>
+    <t>9.5.0. 65+ yrs old</t>
+  </si>
+  <si>
+    <t>1.0. Age</t>
+  </si>
+  <si>
+    <t>2.0. Size of households</t>
+  </si>
+  <si>
+    <t>3.0. Children</t>
+  </si>
+  <si>
+    <t>4.0. Occupation</t>
+  </si>
+  <si>
+    <t>5.0. Affluency</t>
+  </si>
+  <si>
+    <t>6.0. Lifestages</t>
+  </si>
+  <si>
+    <t>7.0. Geographical Area</t>
+  </si>
+  <si>
+    <t>8.0. Income</t>
+  </si>
+  <si>
+    <t>9.0. Age of Baby</t>
+  </si>
+  <si>
+    <t>8.0. POME</t>
+  </si>
+  <si>
+    <t>9.0. Age of Total household</t>
   </si>
 </sst>
 </file>
@@ -593,18 +785,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C388E755-3FE2-45B0-A3F4-E1B5FA8EE619}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,8 +804,11 @@
       <c r="C1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>239528</v>
       </c>
@@ -625,8 +818,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>240386</v>
       </c>
@@ -636,8 +832,11 @@
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>243492</v>
       </c>
@@ -647,8 +846,11 @@
       <c r="C4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>243493</v>
       </c>
@@ -658,8 +860,11 @@
       <c r="C5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>243494</v>
       </c>
@@ -669,8 +874,11 @@
       <c r="C6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>243495</v>
       </c>
@@ -680,8 +888,11 @@
       <c r="C7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>240399</v>
       </c>
@@ -691,8 +902,11 @@
       <c r="C8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>243505</v>
       </c>
@@ -702,8 +916,11 @@
       <c r="C9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>243508</v>
       </c>
@@ -713,8 +930,11 @@
       <c r="C10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>243507</v>
       </c>
@@ -724,8 +944,11 @@
       <c r="C11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>243509</v>
       </c>
@@ -735,8 +958,11 @@
       <c r="C12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>243506</v>
       </c>
@@ -746,8 +972,11 @@
       <c r="C13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>255534</v>
       </c>
@@ -757,8 +986,11 @@
       <c r="C14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>250586</v>
       </c>
@@ -768,8 +1000,11 @@
       <c r="C15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>264341</v>
       </c>
@@ -779,8 +1014,11 @@
       <c r="C16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>264343</v>
       </c>
@@ -790,8 +1028,11 @@
       <c r="C17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>264342</v>
       </c>
@@ -801,8 +1042,11 @@
       <c r="C18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>264322</v>
       </c>
@@ -812,8 +1056,11 @@
       <c r="C19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>257594</v>
       </c>
@@ -823,8 +1070,11 @@
       <c r="C20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>264323</v>
       </c>
@@ -834,8 +1084,11 @@
       <c r="C21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>264324</v>
       </c>
@@ -845,8 +1098,11 @@
       <c r="C22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>264325</v>
       </c>
@@ -856,8 +1112,11 @@
       <c r="C23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>249920</v>
       </c>
@@ -867,8 +1126,11 @@
       <c r="C24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>305885</v>
       </c>
@@ -878,8 +1140,11 @@
       <c r="C25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>264336</v>
       </c>
@@ -889,8 +1154,11 @@
       <c r="C26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>264337</v>
       </c>
@@ -900,8 +1168,11 @@
       <c r="C27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>264338</v>
       </c>
@@ -911,8 +1182,11 @@
       <c r="C28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>243513</v>
       </c>
@@ -922,8 +1196,11 @@
       <c r="C29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>261635</v>
       </c>
@@ -933,8 +1210,11 @@
       <c r="C30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>261636</v>
       </c>
@@ -944,8 +1224,11 @@
       <c r="C31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>261637</v>
       </c>
@@ -955,8 +1238,11 @@
       <c r="C32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>261638</v>
       </c>
@@ -966,8 +1252,11 @@
       <c r="C33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>264332</v>
       </c>
@@ -977,8 +1266,11 @@
       <c r="C34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>243519</v>
       </c>
@@ -988,8 +1280,11 @@
       <c r="C35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>264333</v>
       </c>
@@ -999,8 +1294,11 @@
       <c r="C36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>305884</v>
       </c>
@@ -1010,8 +1308,11 @@
       <c r="C37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>255533</v>
       </c>
@@ -1021,8 +1322,11 @@
       <c r="C38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>273503</v>
       </c>
@@ -1032,8 +1336,11 @@
       <c r="C39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>264340</v>
       </c>
@@ -1043,8 +1350,11 @@
       <c r="C40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>264326</v>
       </c>
@@ -1054,8 +1364,11 @@
       <c r="C41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>264329</v>
       </c>
@@ -1065,8 +1378,11 @@
       <c r="C42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>264328</v>
       </c>
@@ -1076,8 +1392,11 @@
       <c r="C43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>264327</v>
       </c>
@@ -1087,8 +1406,11 @@
       <c r="C44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>264339</v>
       </c>
@@ -1098,8 +1420,11 @@
       <c r="C45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>800001</v>
       </c>
@@ -1109,8 +1434,11 @@
       <c r="C46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>800002</v>
       </c>
@@ -1120,8 +1448,11 @@
       <c r="C47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>800003</v>
       </c>
@@ -1131,8 +1462,11 @@
       <c r="C48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>800004</v>
       </c>
@@ -1142,8 +1476,11 @@
       <c r="C49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>800005</v>
       </c>
@@ -1153,8 +1490,11 @@
       <c r="C50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>800011</v>
       </c>
@@ -1164,8 +1504,11 @@
       <c r="C51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D51" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>800012</v>
       </c>
@@ -1175,8 +1518,11 @@
       <c r="C52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D52" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>800013</v>
       </c>
@@ -1186,8 +1532,11 @@
       <c r="C53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D53" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>800014</v>
       </c>
@@ -1197,8 +1546,11 @@
       <c r="C54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>284329</v>
       </c>
@@ -1208,8 +1560,11 @@
       <c r="C55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D55" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>282145</v>
       </c>
@@ -1219,8 +1574,11 @@
       <c r="C56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>284678</v>
       </c>
@@ -1230,8 +1588,11 @@
       <c r="C57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D57" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>287683</v>
       </c>
@@ -1241,8 +1602,11 @@
       <c r="C58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D58" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>295537</v>
       </c>
@@ -1252,8 +1616,11 @@
       <c r="C59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D59" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>296132</v>
       </c>
@@ -1263,8 +1630,11 @@
       <c r="C60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D60" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>299087</v>
       </c>
@@ -1274,8 +1644,11 @@
       <c r="C61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D61" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>290954</v>
       </c>
@@ -1285,8 +1658,11 @@
       <c r="C62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D62" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>297140</v>
       </c>
@@ -1296,8 +1672,11 @@
       <c r="C63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D63" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>296259</v>
       </c>
@@ -1306,6 +1685,9 @@
       </c>
       <c r="C64">
         <v>63</v>
+      </c>
+      <c r="D64" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>